<commit_message>
Updating database tables excel.
</commit_message>
<xml_diff>
--- a/database_tables.xlsx
+++ b/database_tables.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krjones/Documents/github/mlb2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD1D712C-F0BD-514F-BF64-17CF9B032B70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BCA50A-2CEC-5E48-AB11-C1D458FE229A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15440" windowHeight="17440" xr2:uid="{668117AF-39DF-7B4D-9EB9-8DFBCFEB79A7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15440" windowHeight="17440" activeTab="2" xr2:uid="{668117AF-39DF-7B4D-9EB9-8DFBCFEB79A7}"/>
   </bookViews>
   <sheets>
     <sheet name="games" sheetId="1" r:id="rId1"/>
     <sheet name="mlb_538" sheetId="2" r:id="rId2"/>
     <sheet name="bets" sheetId="3" r:id="rId3"/>
     <sheet name="outcome" sheetId="4" r:id="rId4"/>
+    <sheet name="game_outcome" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -127,6 +128,27 @@
   </si>
   <si>
     <t>outcome</t>
+  </si>
+  <si>
+    <t>a_team</t>
+  </si>
+  <si>
+    <t>h_team</t>
+  </si>
+  <si>
+    <t>a_score</t>
+  </si>
+  <si>
+    <t>h_score</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>winner</t>
   </si>
 </sst>
 </file>
@@ -482,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060EB56E-E6E0-B34F-9BA6-A475A5BF0AC6}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -629,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4111E8E2-1FC6-1549-96D3-1BE2EFA38AC9}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,7 +709,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,4 +741,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECC4355-E79C-8C42-9A5E-66FBB3B140C0}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>